<commit_message>
Write test results to excel file
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buprojects\simplilearn\Assignments\Assignment2\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>pizza</t>
   </si>
@@ -31,12 +31,16 @@
   </si>
   <si>
     <t>Bikanervala</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -348,13 +352,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="false"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -363,6 +370,9 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -370,6 +380,9 @@
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed failed tests due to app change
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -19,18 +19,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>pizza</t>
   </si>
   <si>
-    <t>Domino's Pizza</t>
-  </si>
-  <si>
     <t>chap</t>
   </si>
   <si>
     <t>Bikanervala</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Pizza Pizza</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
   </si>
   <si>
     <t>PASSED</t>
@@ -355,7 +361,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,26 +369,26 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>